<commit_message>
Refactor test scenarios in Excel generation and add helper functions for store values
</commit_message>
<xml_diff>
--- a/test_scenarios.xlsx
+++ b/test_scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Input" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expected Results" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Test Input" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Expected Results" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,12 +629,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Test Produkt A</t>
+          <t>Test Product A</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Size M</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Shoes</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -650,12 +660,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Test Produkt B</t>
+          <t>Test Product B</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Size L</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Bags</t>
         </is>
       </c>
       <c r="O10" t="n">
@@ -677,12 +697,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Test Produkt C</t>
+          <t>Test Product C</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Size S</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Shoes</t>
         </is>
       </c>
     </row>
@@ -695,12 +725,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Test Produkt D</t>
+          <t>Test Product D</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Size XL</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Accessories</t>
         </is>
       </c>
       <c r="L12" t="n">
@@ -749,12 +789,18 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Test Produkt E</t>
+          <t>Test Product E</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Size M</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Shoes</t>
         </is>
       </c>
       <c r="O13" t="n">
@@ -770,7 +816,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Test Produkt F</t>
+          <t>Test Product F</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -778,6 +824,12 @@
           <t>Size L</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="O14" t="n">
         <v>4</v>
       </c>
@@ -794,12 +846,22 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Test Produkt G</t>
+          <t>Test Product G</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>Size S</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>AW24</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Bags</t>
         </is>
       </c>
       <c r="L15" t="n">
@@ -845,16 +907,532 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Test Produkt H</t>
+          <t>Test Product H</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>Size M</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>SS25</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Accessories</t>
         </is>
       </c>
       <c r="X16" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2008</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>MinSize Product 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Size S</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1009</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2009</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>MinSize Product 2</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Size M</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2010</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>MinSize Product 3</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Size S</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1011</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2011</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MinSize Product 3</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Size M</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1012</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2012</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>MinSize Product 3</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Size L</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>MinSize Product 5</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Size XS</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>MinSize Product 5</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Size S</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>MinSize Product 5</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Size M</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>MinSize Product 5</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Size L</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1017</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>MinSize Product 5</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Size XL</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1018</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>MinSize Product Normal</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Size S</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
+      <c r="W27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>MinSize Product Normal</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Size M</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
+      <c r="W28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1020</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>MinSize Product Normal</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Size L</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1021</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>MinSize Product Normal</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Size XL</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Test MinSize</t>
+        </is>
+      </c>
+      <c r="W30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1022</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Edge Case Decimal</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Size M</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Edge Cases</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Edge Case Large</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Size L</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Edge Cases</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>500</v>
+      </c>
+      <c r="W32" t="n">
+        <v>999</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +1446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,127 +1463,127 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Szenario</t>
+          <t>Scenario</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Beschreibung</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Erwartet Script 1 (Stock→Geschäfte)</t>
+          <t>Expected Script 1 (Stock→Stores)</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Erwartet Script 2 (Ausgleich)</t>
+          <t>Expected Script 2 (Balance)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>S1: Stock voll, alle Geschäfte leer</t>
+          <t>S1: Stock full, all stores empty</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Stock=5, alle 0 → verteilt 1 an jeden (max 5 Geschäfte)</t>
+          <t>Stock=5, all 0 → distributes 1 to each (max 5 stores)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>125007=1, 125008=1, 129877=1, 130143=1, 150002=1 (Prio-Reihenfolge)</t>
+          <t>125007=1, 125008=1, 129877=1, 130143=1, 150002=1 (priority order)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Keine Änderung (kein Geschäft &gt;2)</t>
+          <t>No change (no store &gt;2)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>S2: Stock voll, manche Geschäfte haben schon</t>
+          <t>S2: Stock full, some stores already have</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Stock=3, 125007 und 125008 haben schon 1 → nur an leere verteilen</t>
+          <t>Stock=3, 125007 and 125008 already have 1 → only distribute to empty</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>129877=1, 130143=1, 150002=1 (überspringt 125007, 125008)</t>
+          <t>129877=1, 130143=1, 150002=1 (skips 125007, 125008)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Keine Änderung</t>
+          <t>No change</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>S3: Stock leer</t>
+          <t>S3: Stock empty</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Stock=0 → nichts passiert</t>
+          <t>Stock=0 → nothing happens</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Keine Verteilung (Stock=0)</t>
+          <t>No distribution (Stock=0)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Keine Änderung</t>
+          <t>No change</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>S4: Alle Geschäfte voll, Stock hat noch</t>
+          <t>S4: All stores full, Stock still has</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Stock=3, alle haben 1 → Stock bleibt (nichts zu verteilen)</t>
+          <t>Stock=3, all have 1 → Stock remains (nothing to distribute)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Keine Verteilung (alle Geschäfte &gt;0)</t>
+          <t>No distribution (all stores &gt;0)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Keine Änderung (keiner &gt;2)</t>
+          <t>No change (none &gt;2)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>S5: Ein Geschäft hat &gt;2, andere leer</t>
+          <t>S5: One store has &gt;2, others empty</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>125007=5, andere=0 → verteilt Überschuss (5-2=3) an leere</t>
+          <t>125007=5, others=0 → distributes surplus (5-2=3) to empty</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Keine Änderung (Stock=0)</t>
+          <t>No change (Stock=0)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1017,66 +1595,418 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>S6: Mehrere Geschäfte &gt;2, nimmt vom höchsten zuerst</t>
+          <t>S6: Multiple stores &gt;2, takes from highest first</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>125007=4, 125008=6 → nimmt von 125008 zuerst (höchster)</t>
+          <t>125007=4, 125008=6 → takes from 125008 first (highest)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Keine Änderung (Stock=0)</t>
+          <t>No change (Stock=0)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>125008 verteilt 4 (an 129877,130143,150002,125009), dann 125007 verteilt 2 (an 125011,125004)</t>
+          <t>125008 distributes 4 (to 129877,130143,150002,125009), then 125007 distributes 2 (to 125011,125004)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S7: Überschuss geht zu Stock</t>
+          <t>S7: Surplus goes to Stock</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>125007=10, alle anderen haben schon 1 → Rest zu Stock</t>
+          <t>125007=10, all others already have 1 → remainder to Stock</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Keine Änderung (Stock=0, alle &gt;0)</t>
+          <t>No change (Stock=0, all &gt;0)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>125007→Сток=8 (Überschuss 10-2=8, keine leeren Geschäfte)</t>
+          <t>125007→Сток=8 (surplus 10-2=8, no empty stores)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>S8: Фото склад Verteilung</t>
+          <t>S8: Photo Stock Distribution</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Фото склад=3, Stock=0, alle leer → verteilt von Фото</t>
+          <t>Photo Stock=3, Stock=0, all empty → distributes from Photo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mit 'photo': 125007=1, 125008=1, 129877=1</t>
+          <t>With 'photo': 125007=1, 125008=1, 129877=1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Keine Änderung</t>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B1a: MinSize 2 sizes - Size S</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Only 2 sizes in stock → NO transfer (&lt; 3 minimum)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NO transfer - only 2 sizes available</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>B1b: MinSize 2 sizes - Size M</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Only 2 sizes in stock → NO transfer (&lt; 3 minimum)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NO transfer - only 2 sizes available</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>B2a: MinSize 3 sizes - Size S</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Exactly 3 sizes → transfers 3 to first store</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Transfer to 125007 (3 sizes total)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>B2b: MinSize 3 sizes - Size M</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Exactly 3 sizes → transfers 3 to first store</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Transfer to 125007 (3 sizes total)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>B2c: MinSize 3 sizes - Size L</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Exactly 3 sizes → transfers 3 to first store</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Transfer to 125007 (3 sizes total)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>B3a: MinSize 5 sizes - Size XS</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5 sizes available, store has 0 → only 3 transfer</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Only 3 sizes to 125007 (not all 5)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>B3b: MinSize 5 sizes - Size S</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5 sizes available, store has 0 → only 3 transfer</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Only 3 sizes to 125007 (not all 5)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>B3c: MinSize 5 sizes - Size M</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5 sizes available, store has 0 → only 3 transfer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Only 3 sizes to 125007 (not all 5)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>B3d: MinSize 5 sizes - Size L</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5 sizes available, store has 0 → only 3 transfer</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Only 3 sizes to 125007 (not all 5)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>B3e: MinSize 5 sizes - Size XL</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5 sizes available, store has 0 → only 3 transfer</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Only 3 sizes to 125007 (not all 5)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>B4a: Normal rule - Size S (store has)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Store has 2+ sizes → normal rule (not 3-size rule)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Normal rule - L and XL transfer (store has 2+ sizes)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>B4b: Normal rule - Size M (store has)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Store has 2+ sizes → normal rule (not 3-size rule)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Normal rule - L and XL transfer (store has 2+ sizes)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>B4c: Normal rule - Size L (store needs)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Store has 2+ sizes → normal rule, this size transfers</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>This size transfers to 125007</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>B4d: Normal rule - Size XL (store needs)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Store has 2+ sizes → normal rule, this size transfers</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>This size transfers to 125007</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>D1: Decimal numbers</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Stock=3.0, Store=1.0 → should be treated as integers</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Normal processing (decimals → int)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No change</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>D2: Large numbers</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Stock=999, Store=500 → normal processing</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Distributes to stores with 0</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>125007 surplus goes to other stores/Stock</t>
         </is>
       </c>
     </row>

</xml_diff>